<commit_message>
Get more points of Sh-H parabola on left branch
</commit_message>
<xml_diff>
--- a/Shilnikov-Hopf parabola 1.xlsx
+++ b/Shilnikov-Hopf parabola 1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chinsley1\Documents\Dev\PlantChaos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FC9563C8-BF6F-413B-B13A-F66E97BBCC00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66736291-E87C-4D68-9CD2-F50160411D84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{17A6404E-4ABA-4315-9AE8-A49A09E02FB7}"/>
+    <workbookView xWindow="1440" yWindow="1440" windowWidth="16200" windowHeight="9982" xr2:uid="{17A6404E-4ABA-4315-9AE8-A49A09E02FB7}"/>
   </bookViews>
   <sheets>
     <sheet name="Shilnikov-Hopf parabola 1" sheetId="1" r:id="rId1"/>
@@ -52,7 +52,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="185" formatCode="0.000000000000000000000000000"/>
+    <numFmt numFmtId="164" formatCode="0.000000000000000000000000000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -85,7 +85,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="185" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -101,6 +101,1143 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Shilnikov-Hopf parabola 1'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>xshift</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Shilnikov-Hopf parabola 1'!$A$2:$A$49</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="48"/>
+                <c:pt idx="0">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24.000001907348601</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21.999984741210898</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20.000104904174801</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15.0001201629638</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.9999408721923793</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.99983406066894</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.1747685968875801E-4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-5.0000133514404297</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-10.0000391006469</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-14.9998922348022</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-20.0001621246337</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-25.0000095367431</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-26.9999885559082</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-28.999916076660099</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-29.5001621246337</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-29.999994277954102</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-30.499954223632798</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-31.018575668334901</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-31.498464584350501</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-31.9998168945312</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-32.500011444091797</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-32.999988555908203</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-33.500003814697202</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-34</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-34.500049591064403</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-35.000003814697202</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-36.000007629394503</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-36.500038146972599</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>-36.699855804443303</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>-37.000003814697202</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>-37.499996185302699</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>-38.000045776367102</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>-38.499935150146399</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>-39.000049591064403</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>-39.499984741210902</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>-39.999973297119098</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>-40.200000762939403</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>-40.206222534179602</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>-40.237060546875</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>-40.286914825439403</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>-40.400569915771399</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>-40.471832275390597</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>-40.467746734619098</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>-40.455127716064403</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>-40.429866790771399</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>-40.389247894287102</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Shilnikov-Hopf parabola 1'!$B$2:$B$49</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="48"/>
+                <c:pt idx="0">
+                  <c:v>-2.6546171903610198</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-2.63528060913085</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-2.59622979164123</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-2.55641293525695</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-2.4532909393310498</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-2.34562683105468</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-2.2329027652740399</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-2.1151843070983798</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-1.9922280311584399</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-1.86509644985198</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-1.7336276769637999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-1.59937584400177</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-1.465460896492</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-1.41308617591857</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-1.3624629974365201</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-1.35011458396911</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-1.33803367614746</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-1.3261463642120299</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-1.3141053915023799</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-1.3032131195068299</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-1.2921100854873599</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-1.28139436244964</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-1.2711004018783501</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-1.26126408576965</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-1.25197601318359</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-1.2432936429977399</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-1.2353274822235101</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-1.2222155332565301</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-1.2174447774887001</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>-1.21593260765075</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>-1.21420657634735</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>-1.2128483057021999</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>-1.21393430233001</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>-1.21848487854003</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>-1.22810590267181</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>-1.24569404125213</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>-1.2801206111907899</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>-1.3044341802596999</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>-1.3057451248168901</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>-1.3111113309860201</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>-1.32032299041748</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>-1.3500069379806501</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>-1.3997311592102</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>-1.4307007789611801</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>-1.4499776363372801</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>-1.47497522830963</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>-1.5000207424163801</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D6B3-4D89-9422-201BFE8084D1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1203976671"/>
+        <c:axId val="1096533791"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1203976671"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1096533791"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1096533791"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1203976671"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>594370</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>114650</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>634135</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>13104</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{437590B4-D3C5-F293-B1DD-AC97E4C47CE2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -400,10 +1537,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9972971D-D400-474F-85D5-1F740BD0E601}">
-  <dimension ref="A1:K43"/>
+  <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="49" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -753,7 +1890,56 @@
         <v>-1.32032299041748</v>
       </c>
     </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A44">
+        <v>-40.400569915771399</v>
+      </c>
+      <c r="B44">
+        <v>-1.3500069379806501</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A45">
+        <v>-40.471832275390597</v>
+      </c>
+      <c r="B45">
+        <v>-1.3997311592102</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A46">
+        <v>-40.467746734619098</v>
+      </c>
+      <c r="B46">
+        <v>-1.4307007789611801</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A47">
+        <v>-40.455127716064403</v>
+      </c>
+      <c r="B47">
+        <v>-1.4499776363372801</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A48">
+        <v>-40.429866790771399</v>
+      </c>
+      <c r="B48">
+        <v>-1.47497522830963</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A49">
+        <v>-40.389247894287102</v>
+      </c>
+      <c r="B49">
+        <v>-1.5000207424163801</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add lower left points to ShH parabola
</commit_message>
<xml_diff>
--- a/Shilnikov-Hopf parabola 1.xlsx
+++ b/Shilnikov-Hopf parabola 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chinsley1\Documents\Dev\PlantChaos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66736291-E87C-4D68-9CD2-F50160411D84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B742C403-C7FD-4C54-862B-E8AA04897718}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1440" yWindow="1440" windowWidth="16200" windowHeight="9982" xr2:uid="{17A6404E-4ABA-4315-9AE8-A49A09E02FB7}"/>
   </bookViews>
@@ -1539,8 +1539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9972971D-D400-474F-85D5-1F740BD0E601}">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="49" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" zoomScale="49" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>